<commit_message>
gra2005, gsl2008, ssy19 update indexInInstrument in questions and wave in surveys
</commit_message>
<xml_diff>
--- a/data/surveys/surveys.xlsx
+++ b/data/surveys/surveys.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>number</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>annotations.en</t>
+  </si>
+  <si>
+    <t>wave</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -217,6 +220,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -590,167 +599,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
-    <col min="8" max="8" width="64.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1"/>
-    <col min="16" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="64.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1"/>
+    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="17" max="1026" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="192" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="192" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
         <v>24848</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <v>5611</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2" s="6">
         <v>22.6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>27702</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <v>4883</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <v>17.600000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add dataType to survey
</commit_message>
<xml_diff>
--- a/data/surveys/surveys.xlsx
+++ b/data/surveys/surveys.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>number</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>wave</t>
+  </si>
+  <si>
+    <t>dataType.de</t>
+  </si>
+  <si>
+    <t>dataType.en</t>
+  </si>
+  <si>
+    <t>Quantitative Daten</t>
+  </si>
+  <si>
+    <t>Quantitative Data</t>
   </si>
 </sst>
 </file>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +638,7 @@
     <col min="17" max="1026" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,8 +690,14 @@
       <c r="Q1" t="s">
         <v>33</v>
       </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="192" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="192" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -725,8 +743,14 @@
       <c r="O2" s="6">
         <v>22.6</v>
       </c>
+      <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -771,6 +795,12 @@
       </c>
       <c r="O3" s="6">
         <v>17.600000000000001</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
surveys: population.description + population.title
</commit_message>
<xml_diff>
--- a/data/surveys/surveys.xlsx
+++ b/data/surveys/surveys.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>number</t>
   </si>
@@ -36,12 +36,6 @@
   </si>
   <si>
     <t>fieldPeriod.end</t>
-  </si>
-  <si>
-    <t>population.de</t>
-  </si>
-  <si>
-    <t>population.en</t>
   </si>
   <si>
     <t>sample.de</t>
@@ -189,6 +183,24 @@
   </si>
   <si>
     <t>Higher eduaction graduates,  who completed their first professionally recognised degree in the winter semester of 2008-09 or in the summer semester of 2009 at a state approved institution of higher education in the Federal Republic of Germany (with the exception of graduates of German Armed Forces universities, technical universities of administration, dual study programmes, part time or distance learning degree programmes) and who indicated in the main survey of the second wave that they have started a doctorate after their graduation</t>
+  </si>
+  <si>
+    <t>population.description.de</t>
+  </si>
+  <si>
+    <t>population.description.en</t>
+  </si>
+  <si>
+    <t>population.title.de</t>
+  </si>
+  <si>
+    <t>population.title.en</t>
+  </si>
+  <si>
+    <t>Bachelorabsolvent(inn)en und Absolvent(inn)en traditioneller Studiengänge</t>
+  </si>
+  <si>
+    <t>graduates of traditional courses of study and Bachelor graduates</t>
   </si>
 </sst>
 </file>
@@ -270,7 +282,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -304,6 +316,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -675,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,10 +712,13 @@
     <col min="14" max="14" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="1"/>
     <col min="16" max="16" width="18.140625" customWidth="1"/>
-    <col min="17" max="1026" width="10.7109375" customWidth="1"/>
+    <col min="17" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="28.28515625" customWidth="1"/>
+    <col min="22" max="22" width="24" customWidth="1"/>
+    <col min="23" max="1026" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -721,82 +737,88 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="R1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="204" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="204" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="H2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="M2" s="12">
         <v>52550</v>
@@ -808,48 +830,54 @@
         <v>20</v>
       </c>
       <c r="R2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S2" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="204" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="204" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M3" s="12">
         <v>9086</v>
@@ -861,48 +889,54 @@
         <v>52.3</v>
       </c>
       <c r="R3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S3" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="I4" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M4" s="12">
         <v>1136</v>
@@ -914,48 +948,54 @@
         <v>59.5</v>
       </c>
       <c r="R4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S4" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="204" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="204" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7">
         <v>2</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M5" s="12">
         <v>4755</v>
@@ -967,10 +1007,16 @@
         <v>51.8</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S5" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -999,22 +1045,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>